<commit_message>
Fin de proyecto Sálvame
Último commit relacionado al proyecto Sálvame, con los CU08 y CU09 implementados, toda la documentación correspondiente según cronograma y última linea base (3) establecida
</commit_message>
<xml_diff>
--- a/Desarrollo/Salvame/Documentos/Salvame-CP.xlsx
+++ b/Desarrollo/Salvame/Documentos/Salvame-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U-Ramsés\CicloVI\GCS\Repositorio\Desarrollo\Salvame\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5506098-F6AC-41CD-9597-0282521AC154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07CE2CA-8A74-49A8-9467-D13BEB525D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,9 +384,6 @@
     <t>Salvame-MU.docx</t>
   </si>
   <si>
-    <t>Salinas (DP)(A), Rosas(DB)</t>
-  </si>
-  <si>
     <t>Realizar Pruebas finales del Software</t>
   </si>
   <si>
@@ -396,9 +393,6 @@
     <t>Salvame-DPS.docx</t>
   </si>
   <si>
-    <t>Salinas (DP), Rivera(DF),  Mitac(DF), Alata(DF), Ccanto (DF), Camana (DF)</t>
-  </si>
-  <si>
     <t>S9</t>
   </si>
   <si>
@@ -523,6 +517,12 @@
   </si>
   <si>
     <t>Salvame-DEBD.docx</t>
+  </si>
+  <si>
+    <t>Rosas(DB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rivera(DF),  Mitac(DF), Alata(DF), Ccanto (DF), Camana (DF)</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1471,8 @@
   </sheetPr>
   <dimension ref="A1:Z1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1788,7 +1788,7 @@
         <v>38</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>39</v>
@@ -1813,7 +1813,7 @@
         <v>40</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>39</v>
@@ -1838,7 +1838,7 @@
         <v>42</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>39</v>
@@ -1863,7 +1863,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>39</v>
@@ -1888,7 +1888,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>39</v>
@@ -1913,7 +1913,7 @@
         <v>48</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>39</v>
@@ -1938,7 +1938,7 @@
         <v>50</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>39</v>
@@ -1963,7 +1963,7 @@
         <v>52</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>39</v>
@@ -1988,7 +1988,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>39</v>
@@ -2013,7 +2013,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>39</v>
@@ -2040,7 +2040,7 @@
         <v>59</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>60</v>
@@ -2096,7 +2096,7 @@
         <v>67</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>68</v>
@@ -2224,7 +2224,7 @@
         <v>38</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>39</v>
@@ -2251,7 +2251,7 @@
         <v>40</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>39</v>
@@ -2276,7 +2276,7 @@
         <v>42</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E35" s="25" t="s">
         <v>39</v>
@@ -2301,7 +2301,7 @@
         <v>44</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>39</v>
@@ -2326,7 +2326,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>39</v>
@@ -2351,7 +2351,7 @@
         <v>48</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>39</v>
@@ -2376,7 +2376,7 @@
         <v>50</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>39</v>
@@ -2401,7 +2401,7 @@
         <v>52</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>39</v>
@@ -2426,7 +2426,7 @@
         <v>54</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>39</v>
@@ -2451,7 +2451,7 @@
         <v>56</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E42" s="25" t="s">
         <v>39</v>
@@ -2478,7 +2478,7 @@
         <v>59</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>18</v>
@@ -2505,7 +2505,7 @@
         <v>67</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E44" s="52" t="s">
         <v>89</v>
@@ -2696,7 +2696,7 @@
         <v>44879</v>
       </c>
       <c r="H51" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="81" t="s">
         <v>103</v>
@@ -2725,7 +2725,7 @@
         <v>44879</v>
       </c>
       <c r="H52" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="82"/>
       <c r="J52" s="31"/>
@@ -2752,7 +2752,7 @@
         <v>44865</v>
       </c>
       <c r="H53" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="82"/>
       <c r="J53" s="31"/>
@@ -2777,7 +2777,7 @@
         <v>44865</v>
       </c>
       <c r="H54" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="82"/>
       <c r="J54" s="31"/>
@@ -2802,7 +2802,7 @@
         <v>44865</v>
       </c>
       <c r="H55" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="82"/>
       <c r="J55" s="31"/>
@@ -2827,7 +2827,7 @@
         <v>44865</v>
       </c>
       <c r="H56" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="82"/>
       <c r="J56" s="31"/>
@@ -2852,7 +2852,7 @@
         <v>44865</v>
       </c>
       <c r="H57" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="82"/>
       <c r="J57" s="31"/>
@@ -2877,7 +2877,7 @@
         <v>44865</v>
       </c>
       <c r="H58" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="82"/>
       <c r="J58" s="31"/>
@@ -2902,7 +2902,7 @@
         <v>44865</v>
       </c>
       <c r="H59" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="82"/>
       <c r="J59" s="31"/>
@@ -2927,7 +2927,7 @@
         <v>44865</v>
       </c>
       <c r="H60" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" s="82"/>
       <c r="J60" s="31"/>
@@ -2952,7 +2952,7 @@
         <v>44865</v>
       </c>
       <c r="H61" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="82"/>
       <c r="J61" s="31"/>
@@ -2977,13 +2977,13 @@
         <v>44865</v>
       </c>
       <c r="H62" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="82"/>
       <c r="J62" s="31"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" customHeight="1">
+    <row r="63" spans="1:11" ht="24.75" customHeight="1">
       <c r="A63" s="14"/>
       <c r="B63" s="50" t="s">
         <v>87</v>
@@ -2992,7 +2992,7 @@
         <v>59</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E63" s="52" t="s">
         <v>107</v>
@@ -3004,7 +3004,7 @@
         <v>44865</v>
       </c>
       <c r="H63" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="82"/>
       <c r="J63" s="31"/>
@@ -3019,7 +3019,7 @@
         <v>67</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E64" s="52" t="s">
         <v>109</v>
@@ -3031,7 +3031,7 @@
         <v>44865</v>
       </c>
       <c r="H64" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" s="82"/>
       <c r="J64" s="31"/>
@@ -3058,7 +3058,7 @@
         <v>44865</v>
       </c>
       <c r="H65" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="82"/>
       <c r="J65" s="31"/>
@@ -3085,7 +3085,7 @@
         <v>44865</v>
       </c>
       <c r="H66" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" s="82"/>
       <c r="J66" s="31"/>
@@ -3127,7 +3127,7 @@
         <v>44879</v>
       </c>
       <c r="H67" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="82"/>
       <c r="J67" s="31"/>
@@ -3160,7 +3160,7 @@
         <v>117</v>
       </c>
       <c r="E68" s="52" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="F68" s="26">
         <v>44872</v>
@@ -3169,7 +3169,7 @@
         <v>44879</v>
       </c>
       <c r="H68" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" s="82"/>
       <c r="J68" s="31"/>
@@ -3178,16 +3178,16 @@
     <row r="69" spans="1:26" ht="13.5" customHeight="1">
       <c r="A69" s="14"/>
       <c r="B69" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="C69" s="55" t="s">
+      <c r="D69" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D69" s="24" t="s">
-        <v>121</v>
-      </c>
       <c r="E69" s="52" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="F69" s="26">
         <v>44872</v>
@@ -3196,10 +3196,10 @@
         <v>44879</v>
       </c>
       <c r="H69" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" s="81" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J69" s="31"/>
       <c r="K69" s="2"/>
@@ -3216,7 +3216,7 @@
         <v>76</v>
       </c>
       <c r="E70" s="52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F70" s="26">
         <v>44879</v>
@@ -3225,7 +3225,7 @@
         <v>44886</v>
       </c>
       <c r="H70" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="82"/>
       <c r="J70" s="31"/>
@@ -3237,10 +3237,10 @@
         <v>79</v>
       </c>
       <c r="C71" s="55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E71" s="52" t="s">
         <v>82</v>
@@ -3252,10 +3252,10 @@
         <v>44886</v>
       </c>
       <c r="H71" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" s="81" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J71" s="31"/>
       <c r="K71" s="2"/>
@@ -3263,13 +3263,13 @@
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="14"/>
       <c r="B72" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" s="24" t="s">
         <v>128</v>
-      </c>
-      <c r="C72" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>130</v>
       </c>
       <c r="E72" s="52" t="s">
         <v>82</v>
@@ -3281,7 +3281,7 @@
         <v>44886</v>
       </c>
       <c r="H72" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" s="82"/>
       <c r="J72" s="31"/>
@@ -3290,7 +3290,7 @@
     <row r="73" spans="1:26" ht="15.75" customHeight="1">
       <c r="A73" s="14"/>
       <c r="B73" s="63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C73" s="64"/>
       <c r="D73" s="65"/>
@@ -5091,7 +5091,9 @@
   </sheetPr>
   <dimension ref="B1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5103,103 +5105,103 @@
     <row r="1" spans="2:4" ht="15.75" customHeight="1"/>
     <row r="2" spans="2:4" ht="15.75" customHeight="1">
       <c r="B2" s="72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1">
       <c r="B3" s="91" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="92"/>
       <c r="D3" s="89"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" customHeight="1">
       <c r="B4" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="75" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" customHeight="1">
       <c r="B5" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="77" t="s">
         <v>137</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="77" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" customHeight="1">
       <c r="B6" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="77" t="s">
         <v>140</v>
-      </c>
-      <c r="C6" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="77" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" customHeight="1">
       <c r="B7" s="76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D7" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1">
       <c r="B8" s="78" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D8" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" customHeight="1">
       <c r="B9" s="76" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D9" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" customHeight="1">
       <c r="B10" s="76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="77" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" customHeight="1">
       <c r="B11" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="80" t="s">
         <v>150</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="80" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" customHeight="1"/>

</xml_diff>